<commit_message>
Made changes to the pichia_toolkit.xlsx for rectifying the truthy strings error
</commit_message>
<xml_diff>
--- a/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
+++ b/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE9C4B-98A1-D04F-A221-4D8B92CF7AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897CD784-B79A-5349-813D-26E3E1BFDC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7725" uniqueCount="7586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7722" uniqueCount="7583">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22808,12 +22808,6 @@
     <t>F</t>
   </si>
   <si>
-    <t xml:space="preserve">                     TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               FALSE</t>
-  </si>
-  <si>
     <t>SO</t>
   </si>
   <si>
@@ -22821,9 +22815,6 @@
   </si>
   <si>
     <t>Ontology_Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                      TRUE</t>
   </si>
   <si>
     <t>Ontology_Lookup</t>
@@ -69320,7 +69311,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -69345,7 +69336,7 @@
         <v>7552</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>7585</v>
+        <v>7582</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>7553</v>
@@ -69363,7 +69354,7 @@
         <v>7557</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>7583</v>
+        <v>7581</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -69400,11 +69391,11 @@
       <c r="C3" s="31" t="s">
         <v>7559</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>7579</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>7580</v>
+      <c r="D3" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="34" t="b">
+        <v>0</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
@@ -69413,7 +69404,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="35" t="s">
-        <v>7581</v>
+        <v>7579</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -69585,7 +69576,7 @@
         <v>7561</v>
       </c>
       <c r="J9" t="s">
-        <v>7582</v>
+        <v>7580</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -69598,8 +69589,8 @@
       <c r="C10" s="31" t="s">
         <v>7563</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>7584</v>
+      <c r="D10" s="34" t="b">
+        <v>1</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>1</v>
@@ -69617,7 +69608,7 @@
         <v>7561</v>
       </c>
       <c r="J10" t="s">
-        <v>7582</v>
+        <v>7580</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Made changes to the converter_function.py and pichia_toolkit
</commit_message>
<xml_diff>
--- a/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
+++ b/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/tests/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/excel2sbol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897CD784-B79A-5349-813D-26E3E1BFDC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8482D92-8CA6-7A48-B5CC-308C06B4A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69311,7 +69311,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Made changes to the pichia toolkit sheet
</commit_message>
<xml_diff>
--- a/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
+++ b/excel2sbol/excel2sbol/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/excel2sbol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0F4045-F7DA-B946-9390-F9C3F3554DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6FFFCA-04EF-944B-87FB-B527DBDD36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -114,6 +114,7 @@
         <sz val="12"/>
         <color theme="8"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Blue text</t>
     </r>
@@ -123,6 +124,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -132,6 +134,7 @@
         <sz val="12"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>column headers are optional</t>
     </r>
@@ -22824,7 +22827,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22835,53 +22838,63 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF548135"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF548135"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -22889,12 +22902,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -22902,50 +22917,16 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -22957,6 +22938,40 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -23153,7 +23168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23186,8 +23201,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -23465,8 +23479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z97"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23597,12 +23611,12 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -25333,7 +25347,7 @@
       <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -69310,8 +69324,8 @@
   </sheetPr>
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -69335,7 +69349,7 @@
       <c r="C1" s="21" t="s">
         <v>7552</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="21" t="s">
         <v>7582</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -69353,7 +69367,7 @@
       <c r="I1" s="21" t="s">
         <v>7557</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>7581</v>
       </c>
     </row>
@@ -69367,7 +69381,7 @@
       <c r="C2" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D2" s="34" t="b">
+      <c r="D2" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="3" t="b">
@@ -69379,7 +69393,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="35"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
@@ -69391,10 +69405,10 @@
       <c r="C3" s="31" t="s">
         <v>7559</v>
       </c>
-      <c r="D3" s="34" t="b">
+      <c r="D3" s="33" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="34" t="b">
+      <c r="E3" s="33" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="3" t="b">
@@ -69403,7 +69417,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="34" t="s">
         <v>7579</v>
       </c>
     </row>
@@ -69417,7 +69431,7 @@
       <c r="C4" s="22" t="s">
         <v>7563</v>
       </c>
-      <c r="D4" s="34" t="b">
+      <c r="D4" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="b">
@@ -69429,7 +69443,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="35"/>
+      <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
@@ -69441,7 +69455,7 @@
       <c r="C5" s="25" t="s">
         <v>7563</v>
       </c>
-      <c r="D5" s="34" t="b">
+      <c r="D5" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="b">
@@ -69459,7 +69473,7 @@
       <c r="I5" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J5" s="35"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
@@ -69471,7 +69485,7 @@
       <c r="C6" s="25" t="s">
         <v>7568</v>
       </c>
-      <c r="D6" s="34" t="b">
+      <c r="D6" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="b">
@@ -69483,7 +69497,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="35"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
@@ -69495,7 +69509,7 @@
       <c r="C7" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D7" s="34" t="b">
+      <c r="D7" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="b">
@@ -69504,7 +69518,7 @@
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="35"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
@@ -69516,7 +69530,7 @@
       <c r="C8" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D8" s="34" t="b">
+      <c r="D8" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="b">
@@ -69528,7 +69542,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="35"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -69557,7 +69571,7 @@
       <c r="C9" s="25" t="s">
         <v>7563</v>
       </c>
-      <c r="D9" s="34" t="b">
+      <c r="D9" s="33" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="b">
@@ -69589,7 +69603,7 @@
       <c r="C10" s="31" t="s">
         <v>7563</v>
       </c>
-      <c r="D10" s="34" t="b">
+      <c r="D10" s="33" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="b">
@@ -69621,7 +69635,7 @@
       <c r="C11" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D11" s="34" t="b">
+      <c r="D11" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="b">
@@ -69633,7 +69647,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="35"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
@@ -69645,7 +69659,7 @@
       <c r="C12" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D12" s="34" t="b">
+      <c r="D12" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="b">
@@ -69657,7 +69671,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="35"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
@@ -69669,7 +69683,7 @@
       <c r="C13" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D13" s="34" t="b">
+      <c r="D13" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="b">
@@ -69681,7 +69695,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="35"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
@@ -69693,7 +69707,7 @@
       <c r="C14" s="24" t="s">
         <v>7576</v>
       </c>
-      <c r="D14" s="34" t="b">
+      <c r="D14" s="33" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="b">
@@ -69711,7 +69725,7 @@
       <c r="I14" s="3" t="s">
         <v>7578</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>

</xml_diff>